<commit_message>
Match 18 data added. Question 2 added.
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Cricket-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F43F6A-A434-AE43-99F6-1644E49CF60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4E4656-D8B9-4957-A804-1215F7DA3630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21240" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="148">
   <si>
     <t>Match</t>
   </si>
@@ -472,6 +472,12 @@
   </si>
   <si>
     <t>WP Saha</t>
+  </si>
+  <si>
+    <t>M Theekshana</t>
+  </si>
+  <si>
+    <t>MM Ali</t>
   </si>
 </sst>
 </file>
@@ -541,9 +547,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -581,7 +587,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -687,7 +693,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -829,7 +835,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -837,35 +843,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="I49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="7.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="2"/>
+    <col min="4" max="4" width="7.125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="2"/>
+    <col min="9" max="9" width="23.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.375" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.125" style="2" customWidth="1"/>
     <col min="16" max="16" width="13" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="2"/>
+    <col min="17" max="17" width="13.875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -918,7 +924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -971,7 +977,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1024,7 +1030,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1236,7 +1242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1289,7 +1295,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1448,7 +1454,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1554,7 +1560,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -1660,7 +1666,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -1713,7 +1719,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1766,7 +1772,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -1872,7 +1878,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -1925,7 +1931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -1978,7 +1984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -2137,7 +2143,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>7</v>
       </c>
@@ -2190,7 +2196,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -2243,7 +2249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>7</v>
       </c>
@@ -2296,7 +2302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>7</v>
       </c>
@@ -2349,7 +2355,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -2402,7 +2408,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -2455,7 +2461,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>8</v>
       </c>
@@ -2508,7 +2514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>9</v>
       </c>
@@ -2720,7 +2726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -2773,7 +2779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -2826,7 +2832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -2879,7 +2885,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>11</v>
       </c>
@@ -2932,7 +2938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>12</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>12</v>
       </c>
@@ -3038,7 +3044,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>12</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>13</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>14</v>
       </c>
@@ -3197,7 +3203,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>14</v>
       </c>
@@ -3250,7 +3256,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>15</v>
       </c>
@@ -3303,7 +3309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>15</v>
       </c>
@@ -3356,7 +3362,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>15</v>
       </c>
@@ -3409,7 +3415,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>15</v>
       </c>
@@ -3462,7 +3468,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>15</v>
       </c>
@@ -3515,7 +3521,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>16</v>
       </c>
@@ -3568,7 +3574,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>16</v>
       </c>
@@ -3621,7 +3627,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>17</v>
       </c>
@@ -3674,7 +3680,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>17</v>
       </c>
@@ -3727,7 +3733,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>17</v>
       </c>
@@ -3780,7 +3786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>17</v>
       </c>
@@ -3833,7 +3839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>17</v>
       </c>
@@ -3883,6 +3889,165 @@
         <v>102</v>
       </c>
       <c r="Q57" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>18</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="2">
+        <v>2</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="2">
+        <v>10</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>18</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="2">
+        <v>2</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="2">
+        <v>14</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="P59" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>18</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="2">
+        <v>16</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q60" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Day 4 & 5 added
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Cricket-Project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C619468-115A-467A-AFBB-4D1CB50766A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5E4814-3E83-584D-8BB0-6CA0E096F5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21220" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="160">
   <si>
     <t>Match</t>
   </si>
@@ -508,6 +508,12 @@
   </si>
   <si>
     <t>AS Roy</t>
+  </si>
+  <si>
+    <t>RA Tripathi</t>
+  </si>
+  <si>
+    <t>B Kumar</t>
   </si>
 </sst>
 </file>
@@ -577,9 +583,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -617,7 +623,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -723,7 +729,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -865,7 +871,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -873,35 +879,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q70"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="2"/>
-    <col min="4" max="4" width="7.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="7.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.875" style="2"/>
-    <col min="9" max="9" width="23.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="20.875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" style="2" customWidth="1"/>
     <col min="16" max="16" width="13" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.875" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="10.875" style="2"/>
+    <col min="17" max="17" width="13.83203125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,7 +960,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1007,7 +1013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1060,7 +1066,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1113,7 +1119,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1166,7 +1172,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1219,7 +1225,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1325,7 +1331,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1378,7 +1384,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1431,7 +1437,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1537,7 +1543,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1590,7 +1596,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -1749,7 +1755,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -1855,7 +1861,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -1961,7 +1967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -2067,7 +2073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -2120,7 +2126,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>7</v>
       </c>
@@ -2226,7 +2232,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -2279,7 +2285,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>7</v>
       </c>
@@ -2332,7 +2338,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>7</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -2438,7 +2444,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -2491,7 +2497,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>8</v>
       </c>
@@ -2544,7 +2550,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -2703,7 +2709,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>9</v>
       </c>
@@ -2756,7 +2762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -2809,7 +2815,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -2915,7 +2921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>11</v>
       </c>
@@ -2968,7 +2974,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>12</v>
       </c>
@@ -3021,7 +3027,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>12</v>
       </c>
@@ -3074,7 +3080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>12</v>
       </c>
@@ -3127,7 +3133,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>13</v>
       </c>
@@ -3180,7 +3186,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>14</v>
       </c>
@@ -3233,7 +3239,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>14</v>
       </c>
@@ -3286,7 +3292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>15</v>
       </c>
@@ -3339,7 +3345,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>15</v>
       </c>
@@ -3392,7 +3398,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>15</v>
       </c>
@@ -3445,7 +3451,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>15</v>
       </c>
@@ -3498,7 +3504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>15</v>
       </c>
@@ -3551,7 +3557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>16</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>16</v>
       </c>
@@ -3657,7 +3663,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>17</v>
       </c>
@@ -3710,7 +3716,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>17</v>
       </c>
@@ -3763,7 +3769,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>17</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>17</v>
       </c>
@@ -3869,7 +3875,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>17</v>
       </c>
@@ -3922,7 +3928,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>18</v>
       </c>
@@ -3975,7 +3981,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>18</v>
       </c>
@@ -4028,7 +4034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>18</v>
       </c>
@@ -4081,7 +4087,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>19</v>
       </c>
@@ -4134,7 +4140,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>20</v>
       </c>
@@ -4187,7 +4193,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>20</v>
       </c>
@@ -4240,7 +4246,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>20</v>
       </c>
@@ -4293,7 +4299,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>20</v>
       </c>
@@ -4346,7 +4352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>21</v>
       </c>
@@ -4399,7 +4405,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>21</v>
       </c>
@@ -4452,7 +4458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>22</v>
       </c>
@@ -4505,7 +4511,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>22</v>
       </c>
@@ -4558,7 +4564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>22</v>
       </c>
@@ -4608,6 +4614,218 @@
         <v>102</v>
       </c>
       <c r="Q70" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>23</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="2">
+        <v>6</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N71" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O71" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P71" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q71" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>23</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" s="2">
+        <v>10</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N72" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O72" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P72" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q72" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>23</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" s="2">
+        <v>17</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N73" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O73" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="P73" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q73" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>23</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D74" s="2">
+        <v>2</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" s="2">
+        <v>17</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O74" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P74" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q74" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited ReadMe and added new notebooks
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5E4814-3E83-584D-8BB0-6CA0E096F5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95D70B1-447D-B24D-84AD-6A832636AE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21220" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="168">
   <si>
     <t>Match</t>
   </si>
@@ -514,6 +514,30 @@
   </si>
   <si>
     <t>B Kumar</t>
+  </si>
+  <si>
+    <t>Vinod Seshan</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>B Sai Sudharsan</t>
+  </si>
+  <si>
+    <t>KR Sen</t>
+  </si>
+  <si>
+    <t>MS Wade</t>
+  </si>
+  <si>
+    <t>YS Chahal</t>
+  </si>
+  <si>
+    <t>M Shahrukh Khan</t>
+  </si>
+  <si>
+    <t>Avesh Khan</t>
   </si>
 </sst>
 </file>
@@ -879,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" topLeftCell="C49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4829,6 +4853,377 @@
         <v>37</v>
       </c>
     </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
+        <v>24</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G75" s="2">
+        <v>17</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N75" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O75" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="P75" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q75" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
+        <v>24</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G76" s="2">
+        <v>17</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O76" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="P76" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q76" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A77" s="2">
+        <v>24</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G77" s="2">
+        <v>20</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O77" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P77" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>24</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D78" s="2">
+        <v>2</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78" s="2">
+        <v>9</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M78" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N78" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="O78" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P78" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q78" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>24</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" s="2">
+        <v>2</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G79" s="2">
+        <v>11</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="O79" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P79" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q79" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>24</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D80" s="2">
+        <v>2</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G80" s="2">
+        <v>16</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="O80" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P80" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q80" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>24</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D81" s="2">
+        <v>2</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G81" s="2">
+        <v>18</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N81" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="O81" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="P81" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q81" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added april 11 match data
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Cricket-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95D70B1-447D-B24D-84AD-6A832636AE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188C213F-C34F-413C-99A2-716BE8785AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21220" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="175">
   <si>
     <t>Match</t>
   </si>
@@ -538,6 +538,27 @@
   </si>
   <si>
     <t>Avesh Khan</t>
+  </si>
+  <si>
+    <t>RM Patidar</t>
+  </si>
+  <si>
+    <t>JJ Bumrah</t>
+  </si>
+  <si>
+    <t>MK Lomror</t>
+  </si>
+  <si>
+    <t>SA Yadav</t>
+  </si>
+  <si>
+    <t>V Vyshak</t>
+  </si>
+  <si>
+    <t>F du Plessis</t>
+  </si>
+  <si>
+    <t>A Madhwal</t>
   </si>
 </sst>
 </file>
@@ -607,9 +628,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -647,7 +668,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -753,7 +774,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -895,7 +916,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -903,35 +924,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="C62" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="7.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="2"/>
+    <col min="4" max="4" width="7.125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="2"/>
+    <col min="9" max="9" width="23.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.375" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.125" style="2" customWidth="1"/>
     <col min="16" max="16" width="13" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="2"/>
+    <col min="17" max="17" width="13.875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -984,7 +1005,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1037,7 +1058,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1090,7 +1111,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1143,7 +1164,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1196,7 +1217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1249,7 +1270,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1302,7 +1323,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1355,7 +1376,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1408,7 +1429,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1461,7 +1482,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1514,7 +1535,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1567,7 +1588,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1620,7 +1641,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -1673,7 +1694,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -1726,7 +1747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -1779,7 +1800,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1832,7 +1853,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -1885,7 +1906,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -1938,7 +1959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -1991,7 +2012,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -2044,7 +2065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -2097,7 +2118,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -2150,7 +2171,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -2203,7 +2224,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>7</v>
       </c>
@@ -2256,7 +2277,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -2309,7 +2330,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>7</v>
       </c>
@@ -2362,7 +2383,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>7</v>
       </c>
@@ -2415,7 +2436,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -2468,7 +2489,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -2521,7 +2542,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>8</v>
       </c>
@@ -2574,7 +2595,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -2627,7 +2648,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -2680,7 +2701,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -2733,7 +2754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>9</v>
       </c>
@@ -2786,7 +2807,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -2839,7 +2860,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -2892,7 +2913,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -2945,7 +2966,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>11</v>
       </c>
@@ -2998,7 +3019,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>12</v>
       </c>
@@ -3051,7 +3072,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>12</v>
       </c>
@@ -3104,7 +3125,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>12</v>
       </c>
@@ -3157,7 +3178,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>13</v>
       </c>
@@ -3210,7 +3231,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>14</v>
       </c>
@@ -3263,7 +3284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>14</v>
       </c>
@@ -3316,7 +3337,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>15</v>
       </c>
@@ -3369,7 +3390,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>15</v>
       </c>
@@ -3422,7 +3443,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>15</v>
       </c>
@@ -3475,7 +3496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>15</v>
       </c>
@@ -3528,7 +3549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>15</v>
       </c>
@@ -3581,7 +3602,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>16</v>
       </c>
@@ -3634,7 +3655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>16</v>
       </c>
@@ -3687,7 +3708,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>17</v>
       </c>
@@ -3740,7 +3761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>17</v>
       </c>
@@ -3793,7 +3814,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>17</v>
       </c>
@@ -3846,7 +3867,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>17</v>
       </c>
@@ -3899,7 +3920,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>17</v>
       </c>
@@ -3952,7 +3973,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>18</v>
       </c>
@@ -4005,7 +4026,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>18</v>
       </c>
@@ -4058,7 +4079,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>18</v>
       </c>
@@ -4111,7 +4132,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>19</v>
       </c>
@@ -4164,7 +4185,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>20</v>
       </c>
@@ -4217,7 +4238,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>20</v>
       </c>
@@ -4270,7 +4291,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>20</v>
       </c>
@@ -4323,7 +4344,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>20</v>
       </c>
@@ -4376,7 +4397,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>21</v>
       </c>
@@ -4429,7 +4450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>21</v>
       </c>
@@ -4482,7 +4503,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>22</v>
       </c>
@@ -4535,7 +4556,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>22</v>
       </c>
@@ -4588,7 +4609,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>22</v>
       </c>
@@ -4641,7 +4662,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>23</v>
       </c>
@@ -4694,7 +4715,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>23</v>
       </c>
@@ -4747,7 +4768,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>23</v>
       </c>
@@ -4800,7 +4821,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>23</v>
       </c>
@@ -4853,7 +4874,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>24</v>
       </c>
@@ -4906,7 +4927,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>24</v>
       </c>
@@ -4959,7 +4980,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>24</v>
       </c>
@@ -5012,7 +5033,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>24</v>
       </c>
@@ -5065,7 +5086,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>24</v>
       </c>
@@ -5118,7 +5139,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>24</v>
       </c>
@@ -5171,7 +5192,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>24</v>
       </c>
@@ -5221,6 +5242,271 @@
         <v>102</v>
       </c>
       <c r="Q81" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>25</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G82" s="2">
+        <v>11</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N82" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O82" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P82" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q82" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>25</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G83" s="2">
+        <v>16</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M83" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N83" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="O83" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="P83" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q83" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>25</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G84" s="2">
+        <v>17</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N84" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="O84" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P84" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q84" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>25</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G85" s="2">
+        <v>20</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N85" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O85" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="P85" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q85" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>25</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" s="2">
+        <v>2</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86" s="2">
+        <v>14</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M86" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N86" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="P86" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q86" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated drs_data on april 12
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Cricket-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188C213F-C34F-413C-99A2-716BE8785AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7680F938-FE62-4F88-8FD6-397F9192C394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="177">
   <si>
     <t>Match</t>
   </si>
@@ -559,6 +559,12 @@
   </si>
   <si>
     <t>A Madhwal</t>
+  </si>
+  <si>
+    <t>KK Ahmed</t>
+  </si>
+  <si>
+    <t>A Badoni</t>
   </si>
 </sst>
 </file>
@@ -924,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C62" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N85" sqref="N85"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5510,6 +5516,215 @@
         <v>37</v>
       </c>
     </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>26</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G87" s="2">
+        <v>3</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M87" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N87" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="O87" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="P87" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q87" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>26</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G88" s="2">
+        <v>4</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M88" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N88" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O88" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="P88" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q88" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>26</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G89" s="2">
+        <v>10</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M89" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N89" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="O89" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="P89" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>26</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G90" s="2">
+        <v>13</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N90" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="O90" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P90" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q90" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated data till April 18
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Cricket-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C92FCE-4EC6-D747-A278-77AD501D58F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6AAB73-1028-47B5-8DFC-5431E2F34AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21220" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="194">
   <si>
     <t>Match</t>
   </si>
@@ -610,6 +610,12 @@
   </si>
   <si>
     <t>R Powell</t>
+  </si>
+  <si>
+    <t>DA Miller</t>
+  </si>
+  <si>
+    <t>S Sandeep Warrier</t>
   </si>
 </sst>
 </file>
@@ -679,9 +685,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -719,7 +725,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -825,7 +831,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -967,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -975,35 +981,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q116"/>
+  <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C90" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P113" sqref="P113"/>
+    <sheetView tabSelected="1" topLeftCell="G122" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I130" sqref="I130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="7.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="2"/>
+    <col min="4" max="4" width="7.125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="2"/>
+    <col min="9" max="9" width="23.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.375" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.125" style="2" customWidth="1"/>
     <col min="16" max="16" width="13" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="2"/>
+    <col min="17" max="17" width="13.875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1162,7 +1168,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1321,7 +1327,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1480,7 +1486,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1586,7 +1592,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1639,7 +1645,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -1851,7 +1857,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1904,7 +1910,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -1957,7 +1963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -2116,7 +2122,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -2169,7 +2175,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -2222,7 +2228,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -2275,7 +2281,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>7</v>
       </c>
@@ -2328,7 +2334,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -2381,7 +2387,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>7</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>7</v>
       </c>
@@ -2487,7 +2493,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -2540,7 +2546,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>8</v>
       </c>
@@ -2646,7 +2652,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -2699,7 +2705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -2752,7 +2758,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -2805,7 +2811,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>9</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -2911,7 +2917,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -2964,7 +2970,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -3017,7 +3023,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>11</v>
       </c>
@@ -3070,7 +3076,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>12</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>12</v>
       </c>
@@ -3176,7 +3182,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>12</v>
       </c>
@@ -3229,7 +3235,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>13</v>
       </c>
@@ -3282,7 +3288,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>14</v>
       </c>
@@ -3335,7 +3341,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>14</v>
       </c>
@@ -3388,7 +3394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>15</v>
       </c>
@@ -3441,7 +3447,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>15</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>15</v>
       </c>
@@ -3547,7 +3553,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>15</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>15</v>
       </c>
@@ -3653,7 +3659,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>16</v>
       </c>
@@ -3706,7 +3712,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>16</v>
       </c>
@@ -3759,7 +3765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>17</v>
       </c>
@@ -3812,7 +3818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>17</v>
       </c>
@@ -3865,7 +3871,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>17</v>
       </c>
@@ -3918,7 +3924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>17</v>
       </c>
@@ -3971,7 +3977,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>17</v>
       </c>
@@ -4024,7 +4030,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>18</v>
       </c>
@@ -4077,7 +4083,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>18</v>
       </c>
@@ -4130,7 +4136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>18</v>
       </c>
@@ -4183,7 +4189,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>19</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>20</v>
       </c>
@@ -4289,7 +4295,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>20</v>
       </c>
@@ -4342,7 +4348,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>20</v>
       </c>
@@ -4395,7 +4401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>20</v>
       </c>
@@ -4448,7 +4454,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>21</v>
       </c>
@@ -4501,7 +4507,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>21</v>
       </c>
@@ -4554,7 +4560,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>22</v>
       </c>
@@ -4607,7 +4613,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>22</v>
       </c>
@@ -4660,7 +4666,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>22</v>
       </c>
@@ -4713,7 +4719,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>23</v>
       </c>
@@ -4766,7 +4772,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>23</v>
       </c>
@@ -4819,7 +4825,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>23</v>
       </c>
@@ -4872,7 +4878,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>23</v>
       </c>
@@ -4925,7 +4931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>24</v>
       </c>
@@ -4978,7 +4984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>24</v>
       </c>
@@ -5031,7 +5037,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>24</v>
       </c>
@@ -5084,7 +5090,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>24</v>
       </c>
@@ -5137,7 +5143,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>24</v>
       </c>
@@ -5190,7 +5196,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>24</v>
       </c>
@@ -5243,7 +5249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>24</v>
       </c>
@@ -5296,7 +5302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>25</v>
       </c>
@@ -5349,7 +5355,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>25</v>
       </c>
@@ -5402,7 +5408,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>25</v>
       </c>
@@ -5455,7 +5461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>25</v>
       </c>
@@ -5508,7 +5514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>25</v>
       </c>
@@ -5561,7 +5567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>26</v>
       </c>
@@ -5614,7 +5620,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>26</v>
       </c>
@@ -5667,7 +5673,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>26</v>
       </c>
@@ -5720,7 +5726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>26</v>
       </c>
@@ -5773,7 +5779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>27</v>
       </c>
@@ -5826,7 +5832,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>27</v>
       </c>
@@ -5879,7 +5885,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>27</v>
       </c>
@@ -5932,7 +5938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>27</v>
       </c>
@@ -5985,7 +5991,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>27</v>
       </c>
@@ -6038,7 +6044,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>27</v>
       </c>
@@ -6091,7 +6097,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>28</v>
       </c>
@@ -6144,7 +6150,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>28</v>
       </c>
@@ -6197,7 +6203,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>28</v>
       </c>
@@ -6250,7 +6256,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>28</v>
       </c>
@@ -6303,7 +6309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>29</v>
       </c>
@@ -6356,7 +6362,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>29</v>
       </c>
@@ -6409,7 +6415,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>29</v>
       </c>
@@ -6462,7 +6468,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>29</v>
       </c>
@@ -6515,7 +6521,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>30</v>
       </c>
@@ -6568,7 +6574,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>30</v>
       </c>
@@ -6621,7 +6627,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>30</v>
       </c>
@@ -6674,7 +6680,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>30</v>
       </c>
@@ -6727,7 +6733,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>30</v>
       </c>
@@ -6780,7 +6786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>30</v>
       </c>
@@ -6833,7 +6839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>31</v>
       </c>
@@ -6886,7 +6892,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>31</v>
       </c>
@@ -6939,7 +6945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>31</v>
       </c>
@@ -6992,7 +6998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>31</v>
       </c>
@@ -7045,7 +7051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>31</v>
       </c>
@@ -7098,7 +7104,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>31</v>
       </c>
@@ -7148,6 +7154,748 @@
         <v>102</v>
       </c>
       <c r="Q116" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>32</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D117" s="2">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G117" s="2">
+        <v>5</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L117" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M117" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N117" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O117" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="P117" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q117" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>32</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" s="2">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G118" s="2">
+        <v>7</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M118" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N118" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O118" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P118" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q118" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>32</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D119" s="2">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G119" s="2">
+        <v>12</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M119" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N119" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O119" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="P119" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q119" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>32</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D120" s="2">
+        <v>2</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G120" s="2">
+        <v>1</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L120" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M120" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N120" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O120" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="P120" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q120" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>32</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D121" s="2">
+        <v>2</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G121" s="2">
+        <v>3</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L121" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M121" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N121" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O121" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="P121" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q121" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>33</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D122" s="2">
+        <v>1</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G122" s="2">
+        <v>5</v>
+      </c>
+      <c r="H122" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I122" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J122" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K122" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M122" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N122" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O122" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P122" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q122" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>33</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D123" s="2">
+        <v>1</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G123" s="2">
+        <v>15</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I123" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J123" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M123" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N123" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="O123" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="P123" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q123" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>33</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D124" s="2">
+        <v>1</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G124" s="2">
+        <v>16</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M124" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N124" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="O124" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="P124" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q124" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>33</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D125" s="2">
+        <v>1</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G125" s="2">
+        <v>19</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L125" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M125" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N125" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O125" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P125" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q125" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>33</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D126" s="2">
+        <v>1</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G126" s="2">
+        <v>19</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L126" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M126" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N126" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O126" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P126" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q126" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>33</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D127" s="2">
+        <v>1</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G127" s="2">
+        <v>20</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I127" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K127" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L127" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M127" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N127" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O127" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P127" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q127" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>33</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D128" s="2">
+        <v>2</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G128" s="2">
+        <v>2</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I128" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J128" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K128" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L128" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M128" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N128" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="O128" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P128" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q128" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>33</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D129" s="2">
+        <v>2</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G129" s="2">
+        <v>10</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I129" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K129" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L129" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M129" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N129" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O129" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="P129" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q129" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>33</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D130" s="2">
+        <v>2</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G130" s="2">
+        <v>19</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I130" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J130" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K130" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L130" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M130" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N130" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O130" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="P130" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q130" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
april 19 matches updated
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Cricket-Project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6AAB73-1028-47B5-8DFC-5431E2F34AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D2AAD8-2587-864E-ACDA-4D76660F7003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21220" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="196">
   <si>
     <t>Match</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t>S Sandeep Warrier</t>
+  </si>
+  <si>
+    <t>MS Dhoni</t>
+  </si>
+  <si>
+    <t>RA Jadeja</t>
   </si>
 </sst>
 </file>
@@ -685,9 +691,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -725,7 +731,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -831,7 +837,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -973,7 +979,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -981,35 +987,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q130"/>
+  <dimension ref="A1:Q134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G122" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I130" sqref="I130"/>
+    <sheetView tabSelected="1" topLeftCell="C122" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="2"/>
-    <col min="4" max="4" width="7.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="7.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.875" style="2"/>
-    <col min="9" max="9" width="23.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="20.875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" style="2" customWidth="1"/>
     <col min="16" max="16" width="13" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.875" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="10.875" style="2"/>
+    <col min="17" max="17" width="13.83203125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1221,7 +1227,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1380,7 +1386,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1433,7 +1439,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1486,7 +1492,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1698,7 +1704,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -1751,7 +1757,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -1857,7 +1863,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -1963,7 +1969,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -2016,7 +2022,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -2069,7 +2075,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -2122,7 +2128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -2228,7 +2234,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>7</v>
       </c>
@@ -2334,7 +2340,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>7</v>
       </c>
@@ -2440,7 +2446,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>7</v>
       </c>
@@ -2493,7 +2499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -2546,7 +2552,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>8</v>
       </c>
@@ -2652,7 +2658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -2758,7 +2764,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -2811,7 +2817,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>9</v>
       </c>
@@ -2864,7 +2870,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -2917,7 +2923,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -2970,7 +2976,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -3023,7 +3029,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>11</v>
       </c>
@@ -3076,7 +3082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>12</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>12</v>
       </c>
@@ -3182,7 +3188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>12</v>
       </c>
@@ -3235,7 +3241,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>13</v>
       </c>
@@ -3288,7 +3294,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>14</v>
       </c>
@@ -3341,7 +3347,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>14</v>
       </c>
@@ -3394,7 +3400,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>15</v>
       </c>
@@ -3447,7 +3453,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>15</v>
       </c>
@@ -3500,7 +3506,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>15</v>
       </c>
@@ -3553,7 +3559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>15</v>
       </c>
@@ -3606,7 +3612,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>15</v>
       </c>
@@ -3659,7 +3665,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>16</v>
       </c>
@@ -3712,7 +3718,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>16</v>
       </c>
@@ -3765,7 +3771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>17</v>
       </c>
@@ -3818,7 +3824,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>17</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>17</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>17</v>
       </c>
@@ -3977,7 +3983,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>17</v>
       </c>
@@ -4030,7 +4036,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>18</v>
       </c>
@@ -4083,7 +4089,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>18</v>
       </c>
@@ -4136,7 +4142,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>18</v>
       </c>
@@ -4189,7 +4195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>19</v>
       </c>
@@ -4242,7 +4248,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>20</v>
       </c>
@@ -4295,7 +4301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>20</v>
       </c>
@@ -4348,7 +4354,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>20</v>
       </c>
@@ -4401,7 +4407,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>20</v>
       </c>
@@ -4454,7 +4460,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>21</v>
       </c>
@@ -4507,7 +4513,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>21</v>
       </c>
@@ -4560,7 +4566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>22</v>
       </c>
@@ -4613,7 +4619,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>22</v>
       </c>
@@ -4666,7 +4672,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>22</v>
       </c>
@@ -4719,7 +4725,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>23</v>
       </c>
@@ -4772,7 +4778,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>23</v>
       </c>
@@ -4825,7 +4831,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>23</v>
       </c>
@@ -4878,7 +4884,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>23</v>
       </c>
@@ -4931,7 +4937,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>24</v>
       </c>
@@ -4984,7 +4990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>24</v>
       </c>
@@ -5037,7 +5043,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>24</v>
       </c>
@@ -5090,7 +5096,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>24</v>
       </c>
@@ -5143,7 +5149,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>24</v>
       </c>
@@ -5196,7 +5202,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>24</v>
       </c>
@@ -5249,7 +5255,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>24</v>
       </c>
@@ -5302,7 +5308,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>25</v>
       </c>
@@ -5355,7 +5361,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>25</v>
       </c>
@@ -5408,7 +5414,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>25</v>
       </c>
@@ -5461,7 +5467,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>25</v>
       </c>
@@ -5514,7 +5520,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>25</v>
       </c>
@@ -5567,7 +5573,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>26</v>
       </c>
@@ -5620,7 +5626,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>26</v>
       </c>
@@ -5673,7 +5679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>26</v>
       </c>
@@ -5726,7 +5732,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>26</v>
       </c>
@@ -5779,7 +5785,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>27</v>
       </c>
@@ -5832,7 +5838,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>27</v>
       </c>
@@ -5885,7 +5891,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>27</v>
       </c>
@@ -5938,7 +5944,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>27</v>
       </c>
@@ -5991,7 +5997,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>27</v>
       </c>
@@ -6044,7 +6050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>27</v>
       </c>
@@ -6097,7 +6103,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>28</v>
       </c>
@@ -6150,7 +6156,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>28</v>
       </c>
@@ -6203,7 +6209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>28</v>
       </c>
@@ -6256,7 +6262,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>28</v>
       </c>
@@ -6309,7 +6315,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>29</v>
       </c>
@@ -6362,7 +6368,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>29</v>
       </c>
@@ -6415,7 +6421,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>29</v>
       </c>
@@ -6468,7 +6474,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>29</v>
       </c>
@@ -6521,7 +6527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>30</v>
       </c>
@@ -6574,7 +6580,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>30</v>
       </c>
@@ -6627,7 +6633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>30</v>
       </c>
@@ -6680,7 +6686,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>30</v>
       </c>
@@ -6733,7 +6739,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>30</v>
       </c>
@@ -6786,7 +6792,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>30</v>
       </c>
@@ -6839,7 +6845,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>31</v>
       </c>
@@ -6892,7 +6898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>31</v>
       </c>
@@ -6945,7 +6951,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>31</v>
       </c>
@@ -6998,7 +7004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>31</v>
       </c>
@@ -7051,7 +7057,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>31</v>
       </c>
@@ -7104,7 +7110,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>31</v>
       </c>
@@ -7157,7 +7163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>32</v>
       </c>
@@ -7210,7 +7216,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>32</v>
       </c>
@@ -7263,7 +7269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>32</v>
       </c>
@@ -7316,7 +7322,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>32</v>
       </c>
@@ -7369,7 +7375,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>32</v>
       </c>
@@ -7422,7 +7428,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>33</v>
       </c>
@@ -7475,7 +7481,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>33</v>
       </c>
@@ -7528,7 +7534,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>33</v>
       </c>
@@ -7581,7 +7587,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>33</v>
       </c>
@@ -7634,7 +7640,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>33</v>
       </c>
@@ -7687,7 +7693,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>33</v>
       </c>
@@ -7740,7 +7746,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>33</v>
       </c>
@@ -7793,7 +7799,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>33</v>
       </c>
@@ -7846,7 +7852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>33</v>
       </c>
@@ -7896,6 +7902,218 @@
         <v>102</v>
       </c>
       <c r="Q130" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A131" s="2">
+        <v>34</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D131" s="2">
+        <v>1</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G131" s="2">
+        <v>19</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I131" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K131" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L131" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M131" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N131" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="O131" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="P131" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q131" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A132" s="2">
+        <v>34</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" s="2">
+        <v>1</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G132" s="2">
+        <v>19</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I132" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K132" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L132" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M132" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N132" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="O132" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="P132" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q132" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
+        <v>34</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D133" s="2">
+        <v>2</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G133" s="2">
+        <v>18</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I133" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K133" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L133" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M133" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N133" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O133" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="P133" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q133" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A134" s="2">
+        <v>34</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D134" s="2">
+        <v>2</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G134" s="2">
+        <v>19</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I134" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K134" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L134" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M134" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N134" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O134" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="P134" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q134" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated 41st game data and some stats
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA086D7C-122A-0544-8BDF-D76E40D4B878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C6CE48-EDF0-C842-B937-2F5F3DC7DDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21220" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="211">
   <si>
     <t>Match</t>
   </si>
@@ -666,6 +666,9 @@
   </si>
   <si>
     <t>Yash Thakur</t>
+  </si>
+  <si>
+    <t>Swapnil Singh</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q166"/>
+  <dimension ref="A1:Q170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="C162" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O168" sqref="O168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9867,6 +9870,218 @@
         <v>37</v>
       </c>
     </row>
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A167" s="2">
+        <v>41</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D167" s="2">
+        <v>1</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G167" s="2">
+        <v>20</v>
+      </c>
+      <c r="H167" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I167" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J167" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K167" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L167" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M167" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N167" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="O167" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="P167" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q167" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A168" s="2">
+        <v>41</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D168" s="2">
+        <v>2</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G168" s="2">
+        <v>5</v>
+      </c>
+      <c r="H168" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I168" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J168" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K168" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L168" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M168" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N168" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O168" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="P168" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q168" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A169" s="2">
+        <v>41</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D169" s="2">
+        <v>2</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G169" s="2">
+        <v>15</v>
+      </c>
+      <c r="H169" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I169" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J169" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K169" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L169" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M169" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N169" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O169" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="P169" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q169" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A170" s="2">
+        <v>41</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D170" s="2">
+        <v>2</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F170" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G170" s="2">
+        <v>19</v>
+      </c>
+      <c r="H170" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I170" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J170" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K170" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L170" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M170" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N170" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="O170" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P170" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q170" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
data updated till 47 matches
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C6CE48-EDF0-C842-B937-2F5F3DC7DDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAACEA2-4918-B84C-9339-787305847E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21220" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="222">
   <si>
     <t>Match</t>
   </si>
@@ -669,6 +669,39 @@
   </si>
   <si>
     <t>Swapnil Singh</t>
+  </si>
+  <si>
+    <t>RD Chahar</t>
+  </si>
+  <si>
+    <t>PVD Chameera</t>
+  </si>
+  <si>
+    <t>Ramandeep Singh</t>
+  </si>
+  <si>
+    <t>VR Iyer</t>
+  </si>
+  <si>
+    <t>RR Pant</t>
+  </si>
+  <si>
+    <t>Mohammad Nabi</t>
+  </si>
+  <si>
+    <t>Rasikh Salam</t>
+  </si>
+  <si>
+    <t>WG Jacks</t>
+  </si>
+  <si>
+    <t>AM Rahane</t>
+  </si>
+  <si>
+    <t>K Nitish Kumar Reddy</t>
+  </si>
+  <si>
+    <t>PD Salt</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q170"/>
+  <dimension ref="A1:Q192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C162" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O168" sqref="O168"/>
+    <sheetView tabSelected="1" topLeftCell="C155" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P188" sqref="P188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,7 +1099,7 @@
     <col min="12" max="12" width="17.5" style="2" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="20.83203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="2" customWidth="1"/>
     <col min="16" max="16" width="13" style="2" customWidth="1"/>
     <col min="17" max="17" width="13.83203125" style="2" customWidth="1"/>
     <col min="18" max="16384" width="10.83203125" style="2"/>
@@ -10082,6 +10115,1172 @@
         <v>37</v>
       </c>
     </row>
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A171" s="2">
+        <v>42</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D171" s="2">
+        <v>1</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G171" s="2">
+        <v>9</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I171" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J171" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K171" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L171" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M171" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N171" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="O171" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="P171" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q171" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A172" s="2">
+        <v>42</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D172" s="2">
+        <v>1</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F172" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G172" s="2">
+        <v>20</v>
+      </c>
+      <c r="H172" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I172" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J172" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K172" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L172" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M172" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N172" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="O172" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P172" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q172" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A173" s="2">
+        <v>42</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D173" s="2">
+        <v>1</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F173" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G173" s="2">
+        <v>20</v>
+      </c>
+      <c r="H173" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I173" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J173" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K173" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L173" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M173" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N173" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O173" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P173" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q173" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A174" s="2">
+        <v>42</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D174" s="2">
+        <v>2</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G174" s="2">
+        <v>17</v>
+      </c>
+      <c r="H174" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I174" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J174" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K174" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L174" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M174" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N174" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O174" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="P174" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q174" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A175" s="2">
+        <v>42</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D175" s="2">
+        <v>2</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F175" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G175" s="2">
+        <v>18</v>
+      </c>
+      <c r="H175" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I175" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J175" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K175" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L175" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M175" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N175" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O175" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="P175" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q175" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A176" s="2">
+        <v>43</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D176" s="2">
+        <v>1</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F176" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G176" s="2">
+        <v>15</v>
+      </c>
+      <c r="H176" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I176" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J176" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K176" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L176" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M176" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N176" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="O176" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P176" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q176" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A177" s="2">
+        <v>43</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D177" s="2">
+        <v>2</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G177" s="2">
+        <v>11</v>
+      </c>
+      <c r="H177" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I177" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J177" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K177" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L177" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M177" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N177" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O177" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="P177" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q177" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A178" s="2">
+        <v>43</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D178" s="2">
+        <v>2</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G178" s="2">
+        <v>18</v>
+      </c>
+      <c r="H178" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I178" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J178" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K178" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L178" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M178" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N178" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O178" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P178" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q178" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A179" s="2">
+        <v>43</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D179" s="2">
+        <v>2</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G179" s="2">
+        <v>19</v>
+      </c>
+      <c r="H179" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I179" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J179" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K179" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L179" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M179" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N179" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="O179" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="P179" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q179" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A180" s="2">
+        <v>44</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D180" s="2">
+        <v>1</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G180" s="2">
+        <v>19</v>
+      </c>
+      <c r="H180" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I180" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="J180" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K180" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L180" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M180" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N180" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="O180" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="P180" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q180" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A181" s="2">
+        <v>45</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D181" s="2">
+        <v>1</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F181" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G181" s="2">
+        <v>20</v>
+      </c>
+      <c r="H181" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I181" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J181" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K181" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L181" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M181" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N181" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O181" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="P181" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q181" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A182" s="2">
+        <v>45</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D182" s="2">
+        <v>2</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F182" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G182" s="2">
+        <v>7</v>
+      </c>
+      <c r="H182" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I182" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J182" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K182" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L182" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M182" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N182" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="O182" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="P182" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q182" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A183" s="2">
+        <v>45</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183" s="2">
+        <v>2</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G183" s="2">
+        <v>10</v>
+      </c>
+      <c r="H183" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I183" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J183" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K183" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L183" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M183" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N183" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="O183" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="P183" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q183" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A184" s="2">
+        <v>46</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D184" s="2">
+        <v>1</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G184" s="2">
+        <v>2</v>
+      </c>
+      <c r="H184" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I184" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J184" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K184" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L184" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M184" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N184" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="O184" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="P184" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q184" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A185" s="2">
+        <v>46</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D185" s="2">
+        <v>1</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G185" s="2">
+        <v>17</v>
+      </c>
+      <c r="H185" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I185" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J185" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K185" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L185" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M185" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N185" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O185" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="P185" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q185" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A186" s="2">
+        <v>46</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D186" s="2">
+        <v>2</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G186" s="2">
+        <v>17</v>
+      </c>
+      <c r="H186" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I186" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J186" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K186" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L186" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M186" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N186" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O186" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="P186" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q186" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A187" s="2">
+        <v>46</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D187" s="2">
+        <v>2</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G187" s="2">
+        <v>18</v>
+      </c>
+      <c r="H187" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I187" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J187" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K187" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L187" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M187" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N187" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O187" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="P187" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q187" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A188" s="2">
+        <v>47</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D188" s="2">
+        <v>1</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G188" s="2">
+        <v>2</v>
+      </c>
+      <c r="H188" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I188" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J188" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K188" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L188" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M188" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N188" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O188" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P188" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q188" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A189" s="2">
+        <v>47</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D189" s="2">
+        <v>1</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G189" s="2">
+        <v>15</v>
+      </c>
+      <c r="H189" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I189" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J189" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K189" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L189" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M189" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N189" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O189" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="P189" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q189" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A190" s="2">
+        <v>47</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D190" s="2">
+        <v>1</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G190" s="2">
+        <v>18</v>
+      </c>
+      <c r="H190" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I190" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J190" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K190" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L190" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M190" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N190" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O190" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P190" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q190" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A191" s="2">
+        <v>47</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D191" s="2">
+        <v>1</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F191" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G191" s="2">
+        <v>20</v>
+      </c>
+      <c r="H191" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I191" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J191" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K191" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L191" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M191" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N191" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O191" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P191" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q191" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A192" s="2">
+        <v>47</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D192" s="2">
+        <v>2</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G192" s="2">
+        <v>2</v>
+      </c>
+      <c r="H192" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I192" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J192" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K192" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L192" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M192" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N192" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="O192" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="P192" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q192" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
data updated upto May 5
</commit_message>
<xml_diff>
--- a/data/drs_data.xlsx
+++ b/data/drs_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E364E5-6A01-074C-B15A-35B86BE66DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E6F57B-E0AC-A84F-8638-8C33ADD16C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21220" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3069" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="229">
   <si>
     <t>Match</t>
   </si>
@@ -720,6 +720,9 @@
   </si>
   <si>
     <t>MK Pandey</t>
+  </si>
+  <si>
+    <t>DJ Hooda</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q219"/>
+  <dimension ref="A1:Q227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A219" sqref="A219"/>
+    <sheetView tabSelected="1" topLeftCell="C202" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N223" sqref="N223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12730,6 +12733,430 @@
         <v>37</v>
       </c>
     </row>
+    <row r="220" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A220" s="2">
+        <v>53</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D220" s="2">
+        <v>1</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F220" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G220" s="2">
+        <v>9</v>
+      </c>
+      <c r="H220" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I220" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J220" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K220" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L220" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M220" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N220" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O220" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P220" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q220" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="221" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A221" s="2">
+        <v>53</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D221" s="2">
+        <v>2</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F221" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G221" s="2">
+        <v>19</v>
+      </c>
+      <c r="H221" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I221" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J221" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K221" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L221" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M221" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N221" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="O221" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="P221" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q221" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="222" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A222" s="2">
+        <v>54</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D222" s="2">
+        <v>1</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F222" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G222" s="2">
+        <v>15</v>
+      </c>
+      <c r="H222" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I222" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J222" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K222" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L222" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M222" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N222" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O222" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P222" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q222" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="223" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A223" s="2">
+        <v>54</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D223" s="2">
+        <v>1</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F223" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G223" s="2">
+        <v>17</v>
+      </c>
+      <c r="H223" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I223" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J223" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K223" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L223" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M223" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N223" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="O223" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P223" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q223" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="224" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A224" s="2">
+        <v>54</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D224" s="2">
+        <v>1</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F224" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G224" s="2">
+        <v>20</v>
+      </c>
+      <c r="H224" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I224" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J224" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K224" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L224" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M224" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N224" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="O224" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P224" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q224" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A225" s="2">
+        <v>54</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D225" s="2">
+        <v>2</v>
+      </c>
+      <c r="E225" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F225" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G225" s="2">
+        <v>3</v>
+      </c>
+      <c r="H225" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I225" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J225" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K225" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L225" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M225" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N225" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="O225" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P225" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q225" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A226" s="2">
+        <v>54</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D226" s="2">
+        <v>2</v>
+      </c>
+      <c r="E226" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F226" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G226" s="2">
+        <v>9</v>
+      </c>
+      <c r="H226" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I226" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J226" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K226" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L226" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M226" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N226" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="O226" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="P226" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q226" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A227" s="2">
+        <v>54</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D227" s="2">
+        <v>2</v>
+      </c>
+      <c r="E227" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F227" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G227" s="2">
+        <v>17</v>
+      </c>
+      <c r="H227" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I227" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J227" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K227" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L227" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M227" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N227" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O227" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="P227" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q227" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>